<commit_message>
Finished updating paper with recent results
</commit_message>
<xml_diff>
--- a/Labour EPL Paper/analysis_labour_epl_cashflows.xlsx
+++ b/Labour EPL Paper/analysis_labour_epl_cashflows.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ArturoRegalado\Documents\EPL-Analysis\Labour EPL Paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA7AB7F9-0AB1-4A1C-B5E0-7D6156C65F69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD568B3A-8851-4BF8-8EC4-9944D8E94C54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{8D7601BC-8A01-B94E-959E-3CDD7B06B4AA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{8D7601BC-8A01-B94E-959E-3CDD7B06B4AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Oil price - assumption determin" sheetId="9" r:id="rId1"/>
@@ -474,12 +474,6 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
@@ -489,7 +483,13 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -20398,10 +20398,10 @@
                   <c:v>Base EPL</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Labour A</c:v>
+                  <c:v>EPL A</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Labour B</c:v>
+                  <c:v>EPL B</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -20475,10 +20475,10 @@
                   <c:v>Base EPL</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Labour A</c:v>
+                  <c:v>EPL A</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Labour B</c:v>
+                  <c:v>EPL B</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -20552,10 +20552,10 @@
                   <c:v>Base EPL</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Labour A</c:v>
+                  <c:v>EPL A</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Labour B</c:v>
+                  <c:v>EPL B</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -20613,7 +20613,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
+        <c:tickLblPos val="low"/>
         <c:spPr>
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -51608,8 +51608,8 @@
   </sheetPr>
   <dimension ref="E4:AC40"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="Y26" sqref="Y26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -51643,7 +51643,7 @@
       <c r="W6" t="s">
         <v>37</v>
       </c>
-      <c r="X6" s="18">
+      <c r="X6" s="16">
         <f>AA6+NPV(0.1,AA7)</f>
         <v>104</v>
       </c>
@@ -51661,7 +51661,7 @@
       <c r="W7" t="s">
         <v>38</v>
       </c>
-      <c r="X7" s="18">
+      <c r="X7" s="16">
         <f>AB6+NPV(0.1,AB7:AB8)</f>
         <v>343.7355371900826</v>
       </c>
@@ -51688,7 +51688,7 @@
       <c r="W8" t="s">
         <v>39</v>
       </c>
-      <c r="X8" s="18">
+      <c r="X8" s="16">
         <f>AC6+NPV(0.1,AC7:AC9)</f>
         <v>511.93388429752065</v>
       </c>
@@ -51768,25 +51768,25 @@
       <c r="E14" t="s">
         <v>54</v>
       </c>
-      <c r="F14" s="19">
+      <c r="F14" s="17">
         <v>69</v>
       </c>
-      <c r="G14" s="19">
+      <c r="G14" s="17">
         <v>512</v>
       </c>
-      <c r="H14" s="19">
+      <c r="H14" s="17">
         <v>861</v>
       </c>
       <c r="L14" t="s">
         <v>54</v>
       </c>
-      <c r="M14" s="19">
+      <c r="M14" s="17">
         <v>69</v>
       </c>
-      <c r="N14" s="19">
+      <c r="N14" s="17">
         <v>512</v>
       </c>
-      <c r="O14" s="19">
+      <c r="O14" s="17">
         <v>861</v>
       </c>
       <c r="T14" t="s">
@@ -51824,25 +51824,25 @@
       <c r="E15" t="s">
         <v>55</v>
       </c>
-      <c r="F15" s="19">
+      <c r="F15" s="17">
         <v>47</v>
       </c>
-      <c r="G15" s="19">
+      <c r="G15" s="17">
         <v>373</v>
       </c>
-      <c r="H15" s="19">
+      <c r="H15" s="17">
         <v>575</v>
       </c>
       <c r="L15" t="s">
         <v>55</v>
       </c>
-      <c r="M15" s="19">
+      <c r="M15" s="17">
         <v>39</v>
       </c>
-      <c r="N15" s="19">
+      <c r="N15" s="17">
         <v>301</v>
       </c>
-      <c r="O15" s="19">
+      <c r="O15" s="17">
         <v>575</v>
       </c>
       <c r="T15" t="s">
@@ -51880,25 +51880,25 @@
       <c r="E16" t="s">
         <v>56</v>
       </c>
-      <c r="F16" s="19">
+      <c r="F16" s="17">
         <v>49</v>
       </c>
-      <c r="G16" s="19">
+      <c r="G16" s="17">
         <v>425</v>
       </c>
-      <c r="H16" s="19">
+      <c r="H16" s="17">
         <v>758</v>
       </c>
       <c r="L16" t="s">
         <v>56</v>
       </c>
-      <c r="M16" s="19">
+      <c r="M16" s="17">
         <v>5</v>
       </c>
-      <c r="N16" s="19">
+      <c r="N16" s="17">
         <v>235</v>
       </c>
-      <c r="O16" s="19">
+      <c r="O16" s="17">
         <v>514</v>
       </c>
       <c r="T16" t="s">
@@ -51919,11 +51919,11 @@
       <c r="Z16" t="s">
         <v>56</v>
       </c>
-      <c r="AA16" s="20">
+      <c r="AA16" s="18">
         <f>M16/$X$6</f>
         <v>4.807692307692308E-2</v>
       </c>
-      <c r="AB16" s="20">
+      <c r="AB16" s="23">
         <f>N16/$X$7</f>
         <v>0.68366512790921341</v>
       </c>
@@ -51936,31 +51936,31 @@
       <c r="E17" t="s">
         <v>57</v>
       </c>
-      <c r="F17" s="19">
+      <c r="F17" s="17">
         <v>28</v>
       </c>
-      <c r="G17" s="19">
+      <c r="G17" s="17">
         <v>328</v>
       </c>
-      <c r="H17" s="19">
+      <c r="H17" s="17">
         <v>605</v>
       </c>
       <c r="L17" t="s">
         <v>57</v>
       </c>
-      <c r="M17" s="19">
+      <c r="M17" s="17">
         <v>-19</v>
       </c>
-      <c r="N17" s="19">
+      <c r="N17" s="17">
         <v>127</v>
       </c>
-      <c r="O17" s="19">
+      <c r="O17" s="17">
         <v>347</v>
       </c>
       <c r="T17" t="s">
         <v>57</v>
       </c>
-      <c r="U17" s="20">
+      <c r="U17" s="18">
         <f t="shared" si="0"/>
         <v>0.26923076923076922</v>
       </c>
@@ -51975,11 +51975,11 @@
       <c r="Z17" t="s">
         <v>57</v>
       </c>
-      <c r="AA17" s="20">
+      <c r="AA17" s="18">
         <f>M17/$X$6</f>
         <v>-0.18269230769230768</v>
       </c>
-      <c r="AB17" s="20">
+      <c r="AB17" s="18">
         <f>N17/$X$7</f>
         <v>0.36947009040200046</v>
       </c>
@@ -51992,31 +51992,31 @@
       <c r="E18" t="s">
         <v>58</v>
       </c>
-      <c r="F18" s="19">
+      <c r="F18" s="17">
         <v>-11</v>
       </c>
-      <c r="G18" s="19">
+      <c r="G18" s="17">
         <v>200</v>
       </c>
-      <c r="H18" s="19">
+      <c r="H18" s="17">
         <v>416</v>
       </c>
       <c r="L18" t="s">
         <v>58</v>
       </c>
-      <c r="M18" s="19">
+      <c r="M18" s="17">
         <v>-19</v>
       </c>
-      <c r="N18" s="19">
+      <c r="N18" s="17">
         <v>127</v>
       </c>
-      <c r="O18" s="19">
+      <c r="O18" s="17">
         <v>347</v>
       </c>
       <c r="T18" t="s">
         <v>58</v>
       </c>
-      <c r="U18" s="20">
+      <c r="U18" s="18">
         <f t="shared" si="0"/>
         <v>-0.10576923076923077</v>
       </c>
@@ -52031,11 +52031,11 @@
       <c r="Z18" t="s">
         <v>58</v>
       </c>
-      <c r="AA18" s="20">
+      <c r="AA18" s="18">
         <f>M18/$X$6</f>
         <v>-0.18269230769230768</v>
       </c>
-      <c r="AB18" s="20">
+      <c r="AB18" s="18">
         <f>N18/$X$7</f>
         <v>0.36947009040200046</v>
       </c>
@@ -52216,14 +52216,14 @@
       </c>
     </row>
     <row r="33" spans="5:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E33" s="16" t="s">
+      <c r="E33" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="F33" s="16"/>
-      <c r="G33" s="16"/>
-      <c r="H33" s="16"/>
-      <c r="I33" s="16"/>
-      <c r="J33" s="16"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="21"/>
+      <c r="H33" s="21"/>
+      <c r="I33" s="21"/>
+      <c r="J33" s="21"/>
       <c r="M33" t="s">
         <v>37</v>
       </c>
@@ -52235,12 +52235,12 @@
       </c>
     </row>
     <row r="34" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E34" s="16"/>
-      <c r="F34" s="16"/>
-      <c r="G34" s="16"/>
-      <c r="H34" s="16"/>
-      <c r="I34" s="16"/>
-      <c r="J34" s="16"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="21"/>
+      <c r="H34" s="21"/>
+      <c r="I34" s="21"/>
+      <c r="J34" s="21"/>
       <c r="L34" t="s">
         <v>56</v>
       </c>
@@ -52258,12 +52258,12 @@
       </c>
     </row>
     <row r="35" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E35" s="16"/>
-      <c r="F35" s="16"/>
-      <c r="G35" s="16"/>
-      <c r="H35" s="16"/>
-      <c r="I35" s="16"/>
-      <c r="J35" s="16"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="21"/>
+      <c r="G35" s="21"/>
+      <c r="H35" s="21"/>
+      <c r="I35" s="21"/>
+      <c r="J35" s="21"/>
       <c r="L35" t="s">
         <v>57</v>
       </c>
@@ -52377,7 +52377,7 @@
   </sheetPr>
   <dimension ref="B2:W66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+    <sheetView topLeftCell="L18" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
       <selection activeCell="AN36" sqref="AN36"/>
     </sheetView>
   </sheetViews>
@@ -53468,7 +53468,7 @@
       </c>
     </row>
     <row r="46" spans="2:23" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B46" s="23">
+      <c r="B46">
         <v>2025</v>
       </c>
       <c r="C46" s="15">
@@ -53524,7 +53524,7 @@
       </c>
     </row>
     <row r="47" spans="2:23" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B47" s="23">
+      <c r="B47">
         <v>2026</v>
       </c>
       <c r="C47" s="15">
@@ -53580,7 +53580,7 @@
       </c>
     </row>
     <row r="48" spans="2:23" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B48" s="23">
+      <c r="B48">
         <v>2027</v>
       </c>
       <c r="C48" s="15">
@@ -53636,7 +53636,7 @@
       </c>
     </row>
     <row r="49" spans="2:23" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B49" s="23">
+      <c r="B49">
         <v>2028</v>
       </c>
       <c r="C49" s="15">
@@ -53692,7 +53692,7 @@
       </c>
     </row>
     <row r="50" spans="2:23" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B50" s="23">
+      <c r="B50">
         <v>2029</v>
       </c>
       <c r="C50" s="15">
@@ -53748,7 +53748,7 @@
       </c>
     </row>
     <row r="51" spans="2:23" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B51" s="23">
+      <c r="B51">
         <v>2030</v>
       </c>
       <c r="C51" s="15">
@@ -53804,7 +53804,7 @@
       </c>
     </row>
     <row r="52" spans="2:23" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B52" s="23">
+      <c r="B52">
         <v>2031</v>
       </c>
       <c r="C52" s="15">
@@ -53860,7 +53860,7 @@
       </c>
     </row>
     <row r="53" spans="2:23" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B53" s="23">
+      <c r="B53">
         <v>2032</v>
       </c>
       <c r="C53" s="15">
@@ -53916,7 +53916,7 @@
       </c>
     </row>
     <row r="54" spans="2:23" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B54" s="23">
+      <c r="B54">
         <v>2033</v>
       </c>
       <c r="C54" s="15">
@@ -53972,7 +53972,7 @@
       </c>
     </row>
     <row r="55" spans="2:23" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B55" s="23">
+      <c r="B55">
         <v>2034</v>
       </c>
       <c r="C55" s="15">
@@ -54028,7 +54028,7 @@
       </c>
     </row>
     <row r="56" spans="2:23" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B56" s="23">
+      <c r="B56">
         <v>2035</v>
       </c>
       <c r="C56" s="15">
@@ -54330,8 +54330,8 @@
   </sheetPr>
   <dimension ref="F4:R29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="X17" sqref="X17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -54363,64 +54363,64 @@
         <v>56</v>
       </c>
       <c r="K6" t="s">
-        <v>57</v>
+        <v>96</v>
       </c>
       <c r="L6" t="s">
-        <v>58</v>
+        <v>97</v>
       </c>
       <c r="N6" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="7" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="22" t="s">
         <v>79</v>
       </c>
       <c r="G7" t="s">
         <v>25</v>
       </c>
-      <c r="H7" s="19">
+      <c r="H7" s="17">
         <v>70.182474782235843</v>
       </c>
-      <c r="I7" s="19">
+      <c r="I7" s="17">
         <v>48.369917173676484</v>
       </c>
-      <c r="J7" s="19">
+      <c r="J7" s="17">
         <v>49.791209162586775</v>
       </c>
-      <c r="K7" s="19">
+      <c r="K7" s="17">
         <v>28.356844857666943</v>
       </c>
-      <c r="L7" s="19">
+      <c r="L7" s="17">
         <v>-10.414943825626157</v>
       </c>
     </row>
     <row r="8" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F8" s="17"/>
+      <c r="F8" s="22"/>
       <c r="G8" t="s">
         <v>88</v>
       </c>
-      <c r="H8" s="19">
+      <c r="H8" s="17">
         <f>H$7*N8</f>
         <v>63.297784200759637</v>
       </c>
-      <c r="I8" s="19">
-        <f t="shared" ref="I8:M9" si="0">I$7*O8</f>
+      <c r="I8" s="17">
+        <f t="shared" ref="I8:K9" si="0">I$7*O8</f>
         <v>43.292070558777333</v>
       </c>
-      <c r="J8" s="19">
+      <c r="J8" s="17">
         <f t="shared" si="0"/>
         <v>56.822377672088045</v>
       </c>
-      <c r="K8" s="19">
+      <c r="K8" s="17">
         <f t="shared" si="0"/>
         <v>32.13453151586404</v>
       </c>
-      <c r="L8" s="19">
+      <c r="L8" s="17">
         <f>ABS(L$7)*R8 +L7</f>
         <v>8.0440258195813357</v>
       </c>
-      <c r="M8" s="19"/>
+      <c r="M8" s="17"/>
       <c r="N8">
         <v>0.90190299497362814</v>
       </c>
@@ -54438,31 +54438,31 @@
       </c>
     </row>
     <row r="9" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F9" s="17"/>
+      <c r="F9" s="22"/>
       <c r="G9" t="s">
         <v>89</v>
       </c>
-      <c r="H9" s="19">
+      <c r="H9" s="17">
         <f>H$7*N9</f>
         <v>56.415137433832101</v>
       </c>
-      <c r="I9" s="19">
+      <c r="I9" s="17">
         <f t="shared" si="0"/>
         <v>38.584733118339855</v>
       </c>
-      <c r="J9" s="19">
+      <c r="J9" s="17">
         <f t="shared" si="0"/>
         <v>69.857778597399303</v>
       </c>
-      <c r="K9" s="19">
+      <c r="K9" s="17">
         <f t="shared" si="0"/>
         <v>39.30345577623148</v>
       </c>
-      <c r="L9" s="19">
+      <c r="L9" s="17">
         <f>ABS(L$7)*R9 +L7</f>
         <v>20.135731877074402</v>
       </c>
-      <c r="M9" s="19"/>
+      <c r="M9" s="17"/>
       <c r="N9">
         <v>0.8038351113846951</v>
       </c>
@@ -54480,50 +54480,50 @@
       </c>
     </row>
     <row r="11" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F11" s="17" t="s">
+      <c r="F11" s="22" t="s">
         <v>90</v>
       </c>
       <c r="G11" t="s">
         <v>25</v>
       </c>
-      <c r="H11" s="19">
+      <c r="H11" s="17">
         <v>513.22143642620449</v>
       </c>
-      <c r="I11" s="19">
+      <c r="I11" s="17">
         <v>374.85954598578832</v>
       </c>
-      <c r="J11" s="19">
+      <c r="J11" s="17">
         <v>425.76778408194116</v>
       </c>
-      <c r="K11" s="19">
+      <c r="K11" s="17">
         <v>328.06089300742781</v>
       </c>
-      <c r="L11" s="19">
+      <c r="L11" s="17">
         <v>200.61826296208142</v>
       </c>
     </row>
     <row r="12" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F12" s="17"/>
+      <c r="F12" s="22"/>
       <c r="G12" t="s">
         <v>88</v>
       </c>
-      <c r="H12" s="19">
+      <c r="H12" s="17">
         <f>H$11*N12</f>
         <v>458.35030484832015</v>
       </c>
-      <c r="I12" s="19">
+      <c r="I12" s="17">
         <f t="shared" ref="I12:L13" si="1">I$11*O12</f>
         <v>335.74774373664724</v>
       </c>
-      <c r="J12" s="19">
+      <c r="J12" s="17">
         <f t="shared" si="1"/>
         <v>461.35278216656519</v>
       </c>
-      <c r="K12" s="19">
+      <c r="K12" s="17">
         <f t="shared" si="1"/>
         <v>350.519037171062</v>
       </c>
-      <c r="L12" s="19">
+      <c r="L12" s="17">
         <f t="shared" si="1"/>
         <v>227.92281611639046</v>
       </c>
@@ -54544,27 +54544,27 @@
       </c>
     </row>
     <row r="13" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F13" s="17"/>
+      <c r="F13" s="22"/>
       <c r="G13" t="s">
         <v>89</v>
       </c>
-      <c r="H13" s="19">
+      <c r="H13" s="17">
         <f>H$11*N13</f>
         <v>408.51185815358281</v>
       </c>
-      <c r="I13" s="19">
+      <c r="I13" s="17">
         <f t="shared" si="1"/>
         <v>299.24041331251976</v>
       </c>
-      <c r="J13" s="19">
+      <c r="J13" s="17">
         <f t="shared" si="1"/>
         <v>398.57140519888799</v>
       </c>
-      <c r="K13" s="19">
+      <c r="K13" s="17">
         <f t="shared" si="1"/>
         <v>389.3418357922813</v>
       </c>
-      <c r="L13" s="19">
+      <c r="L13" s="17">
         <f t="shared" si="1"/>
         <v>267.8489054670041</v>
       </c>
@@ -54585,50 +54585,50 @@
       </c>
     </row>
     <row r="15" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F15" s="17" t="s">
+      <c r="F15" s="22" t="s">
         <v>81</v>
       </c>
       <c r="G15" t="s">
         <v>25</v>
       </c>
-      <c r="H15" s="19">
+      <c r="H15" s="17">
         <v>864.18890514616066</v>
       </c>
-      <c r="I15" s="19">
+      <c r="I15" s="17">
         <v>578.50141594608601</v>
       </c>
-      <c r="J15" s="19">
+      <c r="J15" s="17">
         <v>759.59448967798824</v>
       </c>
-      <c r="K15" s="19">
+      <c r="K15" s="17">
         <v>607.45157615267647</v>
       </c>
-      <c r="L15" s="19">
+      <c r="L15" s="17">
         <v>417.72201382104407</v>
       </c>
     </row>
     <row r="16" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F16" s="17"/>
+      <c r="F16" s="22"/>
       <c r="G16" t="s">
         <v>88</v>
       </c>
-      <c r="H16" s="19">
+      <c r="H16" s="17">
         <f>H$15*N16</f>
         <v>772.7417701169436</v>
       </c>
-      <c r="I16" s="19">
+      <c r="I16" s="17">
         <f t="shared" ref="I16:L17" si="2">I$15*O16</f>
         <v>517.22304575980172</v>
       </c>
-      <c r="J16" s="19">
+      <c r="J16" s="17">
         <f t="shared" si="2"/>
         <v>700.21055474225864</v>
       </c>
-      <c r="K16" s="19">
+      <c r="K16" s="17">
         <f t="shared" si="2"/>
         <v>640.08298935636913</v>
       </c>
-      <c r="L16" s="19">
+      <c r="L16" s="17">
         <f t="shared" si="2"/>
         <v>458.60429873549225</v>
       </c>
@@ -54649,27 +54649,27 @@
       </c>
     </row>
     <row r="17" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F17" s="17"/>
+      <c r="F17" s="22"/>
       <c r="G17" t="s">
         <v>89</v>
       </c>
-      <c r="H17" s="19">
+      <c r="H17" s="17">
         <f>H$15*N17</f>
         <v>688.71815518444123</v>
       </c>
-      <c r="I17" s="19">
+      <c r="I17" s="17">
         <f t="shared" si="2"/>
         <v>460.98310673779093</v>
       </c>
-      <c r="J17" s="19">
+      <c r="J17" s="17">
         <f t="shared" si="2"/>
         <v>588.88842699109659</v>
       </c>
-      <c r="K17" s="19">
+      <c r="K17" s="17">
         <f t="shared" si="2"/>
         <v>596.21968094472356</v>
       </c>
-      <c r="L17" s="19">
+      <c r="L17" s="17">
         <f t="shared" si="2"/>
         <v>446.66480948151883</v>
       </c>
@@ -54690,70 +54690,70 @@
       </c>
     </row>
     <row r="22" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="G22" s="16" t="s">
+      <c r="G22" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="H22" s="16"/>
-      <c r="I22" s="16"/>
-      <c r="J22" s="16"/>
-      <c r="K22" s="16"/>
-      <c r="L22" s="16"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="21"/>
+      <c r="J22" s="21"/>
+      <c r="K22" s="21"/>
+      <c r="L22" s="21"/>
     </row>
     <row r="23" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="G23" s="16"/>
-      <c r="H23" s="16"/>
-      <c r="I23" s="16"/>
-      <c r="J23" s="16"/>
-      <c r="K23" s="16"/>
-      <c r="L23" s="16"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="21"/>
+      <c r="J23" s="21"/>
+      <c r="K23" s="21"/>
+      <c r="L23" s="21"/>
     </row>
     <row r="24" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="G24" s="16"/>
-      <c r="H24" s="16"/>
-      <c r="I24" s="16"/>
-      <c r="J24" s="16"/>
-      <c r="K24" s="16"/>
-      <c r="L24" s="16"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="21"/>
+      <c r="J24" s="21"/>
+      <c r="K24" s="21"/>
+      <c r="L24" s="21"/>
     </row>
     <row r="25" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="G25" s="16"/>
-      <c r="H25" s="16"/>
-      <c r="I25" s="16"/>
-      <c r="J25" s="16"/>
-      <c r="K25" s="16"/>
-      <c r="L25" s="16"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="21"/>
+      <c r="J25" s="21"/>
+      <c r="K25" s="21"/>
+      <c r="L25" s="21"/>
     </row>
     <row r="26" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="G26" s="16"/>
-      <c r="H26" s="16"/>
-      <c r="I26" s="16"/>
-      <c r="J26" s="16"/>
-      <c r="K26" s="16"/>
-      <c r="L26" s="16"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="21"/>
+      <c r="J26" s="21"/>
+      <c r="K26" s="21"/>
+      <c r="L26" s="21"/>
     </row>
     <row r="27" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="G27" s="16"/>
-      <c r="H27" s="16"/>
-      <c r="I27" s="16"/>
-      <c r="J27" s="16"/>
-      <c r="K27" s="16"/>
-      <c r="L27" s="16"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="21"/>
+      <c r="J27" s="21"/>
+      <c r="K27" s="21"/>
+      <c r="L27" s="21"/>
     </row>
     <row r="28" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="G28" s="16"/>
-      <c r="H28" s="16"/>
-      <c r="I28" s="16"/>
-      <c r="J28" s="16"/>
-      <c r="K28" s="16"/>
-      <c r="L28" s="16"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="21"/>
+      <c r="I28" s="21"/>
+      <c r="J28" s="21"/>
+      <c r="K28" s="21"/>
+      <c r="L28" s="21"/>
     </row>
     <row r="29" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="G29" s="16"/>
-      <c r="H29" s="16"/>
-      <c r="I29" s="16"/>
-      <c r="J29" s="16"/>
-      <c r="K29" s="16"/>
-      <c r="L29" s="16"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="21"/>
+      <c r="I29" s="21"/>
+      <c r="J29" s="21"/>
+      <c r="K29" s="21"/>
+      <c r="L29" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -54774,7 +54774,7 @@
   </sheetPr>
   <dimension ref="B2:BA87"/>
   <sheetViews>
-    <sheetView topLeftCell="AC20" workbookViewId="0">
+    <sheetView topLeftCell="AC1" workbookViewId="0">
       <selection activeCell="AH33" sqref="AH33"/>
     </sheetView>
   </sheetViews>
@@ -56787,20 +56787,20 @@
       </c>
     </row>
     <row r="37" spans="2:53" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="B37" s="21"/>
-      <c r="C37" s="21" t="s">
+      <c r="B37" s="19"/>
+      <c r="C37" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="D37" s="21" t="s">
+      <c r="D37" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="E37" s="21" t="s">
+      <c r="E37" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="F37" s="21" t="s">
+      <c r="F37" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="G37" s="21" t="s">
+      <c r="G37" s="19" t="s">
         <v>75</v>
       </c>
       <c r="J37" s="14"/>
@@ -56885,22 +56885,22 @@
       </c>
     </row>
     <row r="38" spans="2:53" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B38" s="21">
+      <c r="B38" s="19">
         <v>0</v>
       </c>
-      <c r="C38" s="22">
+      <c r="C38" s="20">
         <v>-112</v>
       </c>
-      <c r="D38" s="22">
+      <c r="D38" s="20">
         <v>-67</v>
       </c>
-      <c r="E38" s="22">
+      <c r="E38" s="20">
         <v>-17</v>
       </c>
-      <c r="F38" s="22">
+      <c r="F38" s="20">
         <v>-25</v>
       </c>
-      <c r="G38" s="22">
+      <c r="G38" s="20">
         <v>-67</v>
       </c>
       <c r="J38">
@@ -56947,7 +56947,7 @@
         <v>-112</v>
       </c>
       <c r="AH38" s="15">
-        <f t="shared" ref="AH38:AK52" si="17">D38/$AC5</f>
+        <f t="shared" ref="AH38:AK51" si="17">D38/$AC5</f>
         <v>-67</v>
       </c>
       <c r="AI38" s="15">
@@ -57010,40 +57010,40 @@
       </c>
     </row>
     <row r="39" spans="2:53" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B39" s="21">
+      <c r="B39" s="19">
         <v>1</v>
       </c>
-      <c r="C39" s="22">
+      <c r="C39" s="20">
         <v>-114</v>
       </c>
-      <c r="D39" s="22">
+      <c r="D39" s="20">
         <v>-68</v>
       </c>
-      <c r="E39" s="22">
+      <c r="E39" s="20">
         <v>-17</v>
       </c>
-      <c r="F39" s="22">
+      <c r="F39" s="20">
         <v>-25</v>
       </c>
-      <c r="G39" s="22">
+      <c r="G39" s="20">
         <v>-68</v>
       </c>
       <c r="J39">
         <v>2026</v>
       </c>
-      <c r="K39" s="22">
+      <c r="K39" s="20">
         <v>-112</v>
       </c>
-      <c r="L39" s="22">
+      <c r="L39" s="20">
         <v>-67</v>
       </c>
-      <c r="M39" s="22">
+      <c r="M39" s="20">
         <v>-17</v>
       </c>
-      <c r="N39" s="22">
+      <c r="N39" s="20">
         <v>-25</v>
       </c>
-      <c r="O39" s="22">
+      <c r="O39" s="20">
         <v>-67</v>
       </c>
       <c r="R39">
@@ -57069,7 +57069,7 @@
         <v>2026</v>
       </c>
       <c r="AG39" s="15">
-        <f t="shared" ref="AG39:AG52" si="20">C39/$AC6</f>
+        <f t="shared" ref="AG39:AG51" si="20">C39/$AC6</f>
         <v>-112.094395280236</v>
       </c>
       <c r="AH39" s="15">
@@ -57092,102 +57092,102 @@
         <v>2026</v>
       </c>
       <c r="AO39" s="15">
-        <f t="shared" ref="AO39:AO53" si="21">K39/$AC6</f>
+        <f t="shared" ref="AO39:AO52" si="21">K39/$AC6</f>
         <v>-110.12782694198624</v>
       </c>
       <c r="AP39" s="15">
-        <f t="shared" ref="AP39:AP53" si="22">L39/$AC6</f>
+        <f t="shared" ref="AP39:AP52" si="22">L39/$AC6</f>
         <v>-65.880039331366774</v>
       </c>
       <c r="AQ39" s="15">
-        <f t="shared" ref="AQ39:AQ53" si="23">M39/$AC6</f>
+        <f t="shared" ref="AQ39:AQ52" si="23">M39/$AC6</f>
         <v>-16.715830875122911</v>
       </c>
       <c r="AR39" s="15">
-        <f t="shared" ref="AR39:AR53" si="24">N39/$AC6</f>
+        <f t="shared" ref="AR39:AR52" si="24">N39/$AC6</f>
         <v>-24.582104228121931</v>
       </c>
       <c r="AS39" s="15">
-        <f t="shared" ref="AS39:AS53" si="25">O39/$AC6</f>
+        <f t="shared" ref="AS39:AS52" si="25">O39/$AC6</f>
         <v>-65.880039331366774</v>
       </c>
       <c r="AV39">
         <v>2026</v>
       </c>
       <c r="AW39" s="15">
-        <f t="shared" ref="AW39:AW54" si="26">S39/$AC6</f>
+        <f t="shared" ref="AW39:AW53" si="26">S39/$AC6</f>
         <v>0</v>
       </c>
       <c r="AX39" s="15">
-        <f t="shared" ref="AX39:AX54" si="27">T39/$AC6</f>
+        <f t="shared" ref="AX39:AX53" si="27">T39/$AC6</f>
         <v>0</v>
       </c>
       <c r="AY39" s="15">
-        <f t="shared" ref="AY39:AY54" si="28">U39/$AC6</f>
+        <f t="shared" ref="AY39:AY53" si="28">U39/$AC6</f>
         <v>0</v>
       </c>
       <c r="AZ39" s="15">
-        <f t="shared" ref="AZ39:AZ54" si="29">V39/$AC6</f>
+        <f t="shared" ref="AZ39:AZ53" si="29">V39/$AC6</f>
         <v>0</v>
       </c>
       <c r="BA39" s="15">
-        <f t="shared" ref="BA39:BA54" si="30">W39/$AC6</f>
+        <f t="shared" ref="BA39:BA53" si="30">W39/$AC6</f>
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="2:53" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B40" s="21">
+      <c r="B40" s="19">
         <v>2</v>
       </c>
-      <c r="C40" s="22">
+      <c r="C40" s="20">
         <v>35</v>
       </c>
-      <c r="D40" s="22">
+      <c r="D40" s="20">
         <v>86</v>
       </c>
-      <c r="E40" s="22">
+      <c r="E40" s="20">
         <v>144</v>
       </c>
-      <c r="F40" s="22">
+      <c r="F40" s="20">
         <v>132</v>
       </c>
-      <c r="G40" s="22">
+      <c r="G40" s="20">
         <v>73</v>
       </c>
       <c r="J40">
         <v>2027</v>
       </c>
-      <c r="K40" s="22">
+      <c r="K40" s="20">
         <v>-114</v>
       </c>
-      <c r="L40" s="22">
+      <c r="L40" s="20">
         <v>-68</v>
       </c>
-      <c r="M40" s="22">
+      <c r="M40" s="20">
         <v>-17</v>
       </c>
-      <c r="N40" s="22">
+      <c r="N40" s="20">
         <v>-25</v>
       </c>
-      <c r="O40" s="22">
+      <c r="O40" s="20">
         <v>-68</v>
       </c>
       <c r="R40">
         <v>2027</v>
       </c>
-      <c r="S40" s="22">
+      <c r="S40" s="20">
         <v>-112</v>
       </c>
-      <c r="T40" s="22">
+      <c r="T40" s="20">
         <v>-67</v>
       </c>
-      <c r="U40" s="22">
+      <c r="U40" s="20">
         <v>-17</v>
       </c>
-      <c r="V40" s="22">
+      <c r="V40" s="20">
         <v>-25</v>
       </c>
-      <c r="W40" s="22">
+      <c r="W40" s="20">
         <v>-67</v>
       </c>
       <c r="AF40">
@@ -57261,58 +57261,58 @@
       </c>
     </row>
     <row r="41" spans="2:53" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B41" s="21">
+      <c r="B41" s="19">
         <v>3</v>
       </c>
-      <c r="C41" s="22">
+      <c r="C41" s="20">
         <v>364</v>
       </c>
-      <c r="D41" s="22">
+      <c r="D41" s="20">
         <v>239</v>
       </c>
-      <c r="E41" s="22">
+      <c r="E41" s="20">
         <v>111</v>
       </c>
-      <c r="F41" s="22">
+      <c r="F41" s="20">
         <v>100</v>
       </c>
-      <c r="G41" s="22">
+      <c r="G41" s="20">
         <v>100</v>
       </c>
       <c r="J41">
         <v>2028</v>
       </c>
-      <c r="K41" s="22">
+      <c r="K41" s="20">
         <v>35</v>
       </c>
-      <c r="L41" s="22">
+      <c r="L41" s="20">
         <v>86</v>
       </c>
-      <c r="M41" s="22">
+      <c r="M41" s="20">
         <v>144</v>
       </c>
-      <c r="N41" s="22">
+      <c r="N41" s="20">
         <v>132</v>
       </c>
-      <c r="O41" s="22">
+      <c r="O41" s="20">
         <v>73</v>
       </c>
       <c r="R41">
         <v>2028</v>
       </c>
-      <c r="S41" s="22">
+      <c r="S41" s="20">
         <v>-114</v>
       </c>
-      <c r="T41" s="22">
+      <c r="T41" s="20">
         <v>-68</v>
       </c>
-      <c r="U41" s="22">
+      <c r="U41" s="20">
         <v>-17</v>
       </c>
-      <c r="V41" s="22">
+      <c r="V41" s="20">
         <v>-25</v>
       </c>
-      <c r="W41" s="22">
+      <c r="W41" s="20">
         <v>-68</v>
       </c>
       <c r="AF41">
@@ -57386,58 +57386,58 @@
       </c>
     </row>
     <row r="42" spans="2:53" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B42" s="21">
+      <c r="B42" s="19">
         <v>4</v>
       </c>
-      <c r="C42" s="22">
+      <c r="C42" s="20">
         <v>270</v>
       </c>
-      <c r="D42" s="22">
+      <c r="D42" s="20">
         <v>162</v>
       </c>
-      <c r="E42" s="22">
+      <c r="E42" s="20">
         <v>162</v>
       </c>
-      <c r="F42" s="22">
+      <c r="F42" s="20">
         <v>59</v>
       </c>
-      <c r="G42" s="22">
+      <c r="G42" s="20">
         <v>59</v>
       </c>
       <c r="J42">
         <v>2029</v>
       </c>
-      <c r="K42" s="22">
+      <c r="K42" s="20">
         <v>364</v>
       </c>
-      <c r="L42" s="22">
+      <c r="L42" s="20">
         <v>239</v>
       </c>
-      <c r="M42" s="22">
+      <c r="M42" s="20">
         <v>111</v>
       </c>
-      <c r="N42" s="22">
+      <c r="N42" s="20">
         <v>100</v>
       </c>
-      <c r="O42" s="22">
+      <c r="O42" s="20">
         <v>100</v>
       </c>
       <c r="R42">
         <v>2029</v>
       </c>
-      <c r="S42" s="22">
+      <c r="S42" s="20">
         <v>35</v>
       </c>
-      <c r="T42" s="22">
+      <c r="T42" s="20">
         <v>86</v>
       </c>
-      <c r="U42" s="22">
+      <c r="U42" s="20">
         <v>144</v>
       </c>
-      <c r="V42" s="22">
+      <c r="V42" s="20">
         <v>132</v>
       </c>
-      <c r="W42" s="22">
+      <c r="W42" s="20">
         <v>73</v>
       </c>
       <c r="AF42">
@@ -57511,58 +57511,58 @@
       </c>
     </row>
     <row r="43" spans="2:53" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B43" s="21">
+      <c r="B43" s="19">
         <v>5</v>
       </c>
-      <c r="C43" s="22">
+      <c r="C43" s="20">
         <v>198</v>
       </c>
-      <c r="D43" s="22">
+      <c r="D43" s="20">
         <v>119</v>
       </c>
-      <c r="E43" s="22">
+      <c r="E43" s="20">
         <v>119</v>
       </c>
-      <c r="F43" s="22">
+      <c r="F43" s="20">
         <v>119</v>
       </c>
-      <c r="G43" s="22">
+      <c r="G43" s="20">
         <v>119</v>
       </c>
       <c r="J43">
         <v>2030</v>
       </c>
-      <c r="K43" s="22">
+      <c r="K43" s="20">
         <v>270</v>
       </c>
-      <c r="L43" s="22">
+      <c r="L43" s="20">
         <v>162</v>
       </c>
-      <c r="M43" s="22">
+      <c r="M43" s="20">
         <v>162</v>
       </c>
-      <c r="N43" s="22">
+      <c r="N43" s="20">
         <v>59</v>
       </c>
-      <c r="O43" s="22">
+      <c r="O43" s="20">
         <v>59</v>
       </c>
       <c r="R43">
         <v>2030</v>
       </c>
-      <c r="S43" s="22">
+      <c r="S43" s="20">
         <v>364</v>
       </c>
-      <c r="T43" s="22">
+      <c r="T43" s="20">
         <v>239</v>
       </c>
-      <c r="U43" s="22">
+      <c r="U43" s="20">
         <v>111</v>
       </c>
-      <c r="V43" s="22">
+      <c r="V43" s="20">
         <v>100</v>
       </c>
-      <c r="W43" s="22">
+      <c r="W43" s="20">
         <v>100</v>
       </c>
       <c r="AF43">
@@ -57636,58 +57636,58 @@
       </c>
     </row>
     <row r="44" spans="2:53" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B44" s="21">
+      <c r="B44" s="19">
         <v>6</v>
       </c>
-      <c r="C44" s="22">
+      <c r="C44" s="20">
         <v>143</v>
       </c>
-      <c r="D44" s="22">
+      <c r="D44" s="20">
         <v>86</v>
       </c>
-      <c r="E44" s="22">
+      <c r="E44" s="20">
         <v>86</v>
       </c>
-      <c r="F44" s="22">
+      <c r="F44" s="20">
         <v>86</v>
       </c>
-      <c r="G44" s="22">
+      <c r="G44" s="20">
         <v>86</v>
       </c>
       <c r="J44">
         <v>2031</v>
       </c>
-      <c r="K44" s="22">
+      <c r="K44" s="20">
         <v>198</v>
       </c>
-      <c r="L44" s="22">
+      <c r="L44" s="20">
         <v>119</v>
       </c>
-      <c r="M44" s="22">
+      <c r="M44" s="20">
         <v>119</v>
       </c>
-      <c r="N44" s="22">
+      <c r="N44" s="20">
         <v>119</v>
       </c>
-      <c r="O44" s="22">
+      <c r="O44" s="20">
         <v>119</v>
       </c>
       <c r="R44">
         <v>2031</v>
       </c>
-      <c r="S44" s="22">
+      <c r="S44" s="20">
         <v>270</v>
       </c>
-      <c r="T44" s="22">
+      <c r="T44" s="20">
         <v>162</v>
       </c>
-      <c r="U44" s="22">
+      <c r="U44" s="20">
         <v>162</v>
       </c>
-      <c r="V44" s="22">
+      <c r="V44" s="20">
         <v>59</v>
       </c>
-      <c r="W44" s="22">
+      <c r="W44" s="20">
         <v>59</v>
       </c>
       <c r="AF44">
@@ -57761,58 +57761,58 @@
       </c>
     </row>
     <row r="45" spans="2:53" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B45" s="21">
+      <c r="B45" s="19">
         <v>7</v>
       </c>
-      <c r="C45" s="22">
+      <c r="C45" s="20">
         <v>101</v>
       </c>
-      <c r="D45" s="22">
+      <c r="D45" s="20">
         <v>61</v>
       </c>
-      <c r="E45" s="22">
+      <c r="E45" s="20">
         <v>61</v>
       </c>
-      <c r="F45" s="22">
+      <c r="F45" s="20">
         <v>61</v>
       </c>
-      <c r="G45" s="22">
+      <c r="G45" s="20">
         <v>61</v>
       </c>
       <c r="J45">
         <v>2032</v>
       </c>
-      <c r="K45" s="22">
+      <c r="K45" s="20">
         <v>143</v>
       </c>
-      <c r="L45" s="22">
+      <c r="L45" s="20">
         <v>86</v>
       </c>
-      <c r="M45" s="22">
+      <c r="M45" s="20">
         <v>86</v>
       </c>
-      <c r="N45" s="22">
+      <c r="N45" s="20">
         <v>86</v>
       </c>
-      <c r="O45" s="22">
+      <c r="O45" s="20">
         <v>86</v>
       </c>
       <c r="R45">
         <v>2032</v>
       </c>
-      <c r="S45" s="22">
+      <c r="S45" s="20">
         <v>198</v>
       </c>
-      <c r="T45" s="22">
+      <c r="T45" s="20">
         <v>119</v>
       </c>
-      <c r="U45" s="22">
+      <c r="U45" s="20">
         <v>119</v>
       </c>
-      <c r="V45" s="22">
+      <c r="V45" s="20">
         <v>119</v>
       </c>
-      <c r="W45" s="22">
+      <c r="W45" s="20">
         <v>119</v>
       </c>
       <c r="AF45">
@@ -57886,58 +57886,58 @@
       </c>
     </row>
     <row r="46" spans="2:53" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B46" s="21">
+      <c r="B46" s="19">
         <v>8</v>
       </c>
-      <c r="C46" s="22">
+      <c r="C46" s="20">
         <v>68</v>
       </c>
-      <c r="D46" s="22">
+      <c r="D46" s="20">
         <v>41</v>
       </c>
-      <c r="E46" s="22">
+      <c r="E46" s="20">
         <v>41</v>
       </c>
-      <c r="F46" s="22">
+      <c r="F46" s="20">
         <v>41</v>
       </c>
-      <c r="G46" s="22">
+      <c r="G46" s="20">
         <v>41</v>
       </c>
       <c r="J46">
         <v>2033</v>
       </c>
-      <c r="K46" s="22">
+      <c r="K46" s="20">
         <v>101</v>
       </c>
-      <c r="L46" s="22">
+      <c r="L46" s="20">
         <v>61</v>
       </c>
-      <c r="M46" s="22">
+      <c r="M46" s="20">
         <v>61</v>
       </c>
-      <c r="N46" s="22">
+      <c r="N46" s="20">
         <v>61</v>
       </c>
-      <c r="O46" s="22">
+      <c r="O46" s="20">
         <v>61</v>
       </c>
       <c r="R46">
         <v>2033</v>
       </c>
-      <c r="S46" s="22">
+      <c r="S46" s="20">
         <v>143</v>
       </c>
-      <c r="T46" s="22">
+      <c r="T46" s="20">
         <v>86</v>
       </c>
-      <c r="U46" s="22">
+      <c r="U46" s="20">
         <v>86</v>
       </c>
-      <c r="V46" s="22">
+      <c r="V46" s="20">
         <v>86</v>
       </c>
-      <c r="W46" s="22">
+      <c r="W46" s="20">
         <v>86</v>
       </c>
       <c r="AF46">
@@ -58011,58 +58011,58 @@
       </c>
     </row>
     <row r="47" spans="2:53" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B47" s="21">
+      <c r="B47" s="19">
         <v>9</v>
       </c>
-      <c r="C47" s="22">
+      <c r="C47" s="20">
         <v>43</v>
       </c>
-      <c r="D47" s="22">
+      <c r="D47" s="20">
         <v>26</v>
       </c>
-      <c r="E47" s="22">
+      <c r="E47" s="20">
         <v>26</v>
       </c>
-      <c r="F47" s="22">
+      <c r="F47" s="20">
         <v>26</v>
       </c>
-      <c r="G47" s="22">
+      <c r="G47" s="20">
         <v>26</v>
       </c>
       <c r="J47">
         <v>2034</v>
       </c>
-      <c r="K47" s="22">
+      <c r="K47" s="20">
         <v>68</v>
       </c>
-      <c r="L47" s="22">
+      <c r="L47" s="20">
         <v>41</v>
       </c>
-      <c r="M47" s="22">
+      <c r="M47" s="20">
         <v>41</v>
       </c>
-      <c r="N47" s="22">
+      <c r="N47" s="20">
         <v>41</v>
       </c>
-      <c r="O47" s="22">
+      <c r="O47" s="20">
         <v>41</v>
       </c>
       <c r="R47">
         <v>2034</v>
       </c>
-      <c r="S47" s="22">
+      <c r="S47" s="20">
         <v>101</v>
       </c>
-      <c r="T47" s="22">
+      <c r="T47" s="20">
         <v>61</v>
       </c>
-      <c r="U47" s="22">
+      <c r="U47" s="20">
         <v>61</v>
       </c>
-      <c r="V47" s="22">
+      <c r="V47" s="20">
         <v>61</v>
       </c>
-      <c r="W47" s="22">
+      <c r="W47" s="20">
         <v>61</v>
       </c>
       <c r="AF47">
@@ -58136,58 +58136,58 @@
       </c>
     </row>
     <row r="48" spans="2:53" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B48" s="21">
+      <c r="B48" s="19">
         <v>10</v>
       </c>
-      <c r="C48" s="22">
+      <c r="C48" s="20">
         <v>24</v>
       </c>
-      <c r="D48" s="22">
+      <c r="D48" s="20">
         <v>14</v>
       </c>
-      <c r="E48" s="22">
+      <c r="E48" s="20">
         <v>14</v>
       </c>
-      <c r="F48" s="22">
+      <c r="F48" s="20">
         <v>14</v>
       </c>
-      <c r="G48" s="22">
+      <c r="G48" s="20">
         <v>14</v>
       </c>
       <c r="J48">
         <v>2035</v>
       </c>
-      <c r="K48" s="22">
+      <c r="K48" s="20">
         <v>43</v>
       </c>
-      <c r="L48" s="22">
+      <c r="L48" s="20">
         <v>26</v>
       </c>
-      <c r="M48" s="22">
+      <c r="M48" s="20">
         <v>26</v>
       </c>
-      <c r="N48" s="22">
+      <c r="N48" s="20">
         <v>26</v>
       </c>
-      <c r="O48" s="22">
+      <c r="O48" s="20">
         <v>26</v>
       </c>
       <c r="R48">
         <v>2035</v>
       </c>
-      <c r="S48" s="22">
+      <c r="S48" s="20">
         <v>68</v>
       </c>
-      <c r="T48" s="22">
+      <c r="T48" s="20">
         <v>41</v>
       </c>
-      <c r="U48" s="22">
+      <c r="U48" s="20">
         <v>41</v>
       </c>
-      <c r="V48" s="22">
+      <c r="V48" s="20">
         <v>41</v>
       </c>
-      <c r="W48" s="22">
+      <c r="W48" s="20">
         <v>41</v>
       </c>
       <c r="AF48">
@@ -58261,58 +58261,58 @@
       </c>
     </row>
     <row r="49" spans="2:53" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B49" s="21">
+      <c r="B49" s="19">
         <v>11</v>
       </c>
-      <c r="C49" s="22">
+      <c r="C49" s="20">
         <v>9</v>
       </c>
-      <c r="D49" s="22">
+      <c r="D49" s="20">
         <v>5</v>
       </c>
-      <c r="E49" s="22">
+      <c r="E49" s="20">
         <v>5</v>
       </c>
-      <c r="F49" s="22">
+      <c r="F49" s="20">
         <v>5</v>
       </c>
-      <c r="G49" s="22">
+      <c r="G49" s="20">
         <v>5</v>
       </c>
       <c r="J49">
         <v>2036</v>
       </c>
-      <c r="K49" s="22">
+      <c r="K49" s="20">
         <v>24</v>
       </c>
-      <c r="L49" s="22">
+      <c r="L49" s="20">
         <v>14</v>
       </c>
-      <c r="M49" s="22">
+      <c r="M49" s="20">
         <v>14</v>
       </c>
-      <c r="N49" s="22">
+      <c r="N49" s="20">
         <v>14</v>
       </c>
-      <c r="O49" s="22">
+      <c r="O49" s="20">
         <v>14</v>
       </c>
       <c r="R49">
         <v>2036</v>
       </c>
-      <c r="S49" s="22">
+      <c r="S49" s="20">
         <v>43</v>
       </c>
-      <c r="T49" s="22">
+      <c r="T49" s="20">
         <v>26</v>
       </c>
-      <c r="U49" s="22">
+      <c r="U49" s="20">
         <v>26</v>
       </c>
-      <c r="V49" s="22">
+      <c r="V49" s="20">
         <v>26</v>
       </c>
-      <c r="W49" s="22">
+      <c r="W49" s="20">
         <v>26</v>
       </c>
       <c r="AF49">
@@ -58386,58 +58386,58 @@
       </c>
     </row>
     <row r="50" spans="2:53" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B50" s="21">
+      <c r="B50" s="19">
         <v>12</v>
       </c>
-      <c r="C50" s="22">
+      <c r="C50" s="20">
         <v>-3</v>
       </c>
-      <c r="D50" s="22">
+      <c r="D50" s="20">
         <v>-3</v>
       </c>
-      <c r="E50" s="22">
+      <c r="E50" s="20">
         <v>-3</v>
       </c>
-      <c r="F50" s="22">
+      <c r="F50" s="20">
         <v>-3</v>
       </c>
-      <c r="G50" s="22">
+      <c r="G50" s="20">
         <v>-3</v>
       </c>
       <c r="J50">
         <v>2037</v>
       </c>
-      <c r="K50" s="22">
+      <c r="K50" s="20">
         <v>9</v>
       </c>
-      <c r="L50" s="22">
+      <c r="L50" s="20">
         <v>5</v>
       </c>
-      <c r="M50" s="22">
+      <c r="M50" s="20">
         <v>5</v>
       </c>
-      <c r="N50" s="22">
+      <c r="N50" s="20">
         <v>5</v>
       </c>
-      <c r="O50" s="22">
+      <c r="O50" s="20">
         <v>5</v>
       </c>
       <c r="R50">
         <v>2037</v>
       </c>
-      <c r="S50" s="22">
+      <c r="S50" s="20">
         <v>24</v>
       </c>
-      <c r="T50" s="22">
+      <c r="T50" s="20">
         <v>14</v>
       </c>
-      <c r="U50" s="22">
+      <c r="U50" s="20">
         <v>14</v>
       </c>
-      <c r="V50" s="22">
+      <c r="V50" s="20">
         <v>14</v>
       </c>
-      <c r="W50" s="22">
+      <c r="W50" s="20">
         <v>14</v>
       </c>
       <c r="AF50">
@@ -58511,58 +58511,58 @@
       </c>
     </row>
     <row r="51" spans="2:53" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B51" s="21">
+      <c r="B51" s="19">
         <v>13</v>
       </c>
-      <c r="C51" s="22">
+      <c r="C51" s="20">
         <v>-48</v>
       </c>
-      <c r="D51" s="22">
+      <c r="D51" s="20">
         <v>-29</v>
       </c>
-      <c r="E51" s="22">
+      <c r="E51" s="20">
         <v>-29</v>
       </c>
-      <c r="F51" s="22">
+      <c r="F51" s="20">
         <v>-29</v>
       </c>
-      <c r="G51" s="22">
+      <c r="G51" s="20">
         <v>-29</v>
       </c>
       <c r="J51">
         <v>2038</v>
       </c>
-      <c r="K51" s="22">
+      <c r="K51" s="20">
         <v>-3</v>
       </c>
-      <c r="L51" s="22">
+      <c r="L51" s="20">
         <v>-3</v>
       </c>
-      <c r="M51" s="22">
+      <c r="M51" s="20">
         <v>-3</v>
       </c>
-      <c r="N51" s="22">
+      <c r="N51" s="20">
         <v>-3</v>
       </c>
-      <c r="O51" s="22">
+      <c r="O51" s="20">
         <v>-3</v>
       </c>
       <c r="R51">
         <v>2038</v>
       </c>
-      <c r="S51" s="22">
+      <c r="S51" s="20">
         <v>9</v>
       </c>
-      <c r="T51" s="22">
+      <c r="T51" s="20">
         <v>5</v>
       </c>
-      <c r="U51" s="22">
+      <c r="U51" s="20">
         <v>5</v>
       </c>
-      <c r="V51" s="22">
+      <c r="V51" s="20">
         <v>5</v>
       </c>
-      <c r="W51" s="22">
+      <c r="W51" s="20">
         <v>5</v>
       </c>
       <c r="AF51">
@@ -58644,37 +58644,37 @@
       <c r="J52">
         <v>2039</v>
       </c>
-      <c r="K52" s="22">
+      <c r="K52" s="20">
         <v>-48</v>
       </c>
-      <c r="L52" s="22">
+      <c r="L52" s="20">
         <v>-29</v>
       </c>
-      <c r="M52" s="22">
+      <c r="M52" s="20">
         <v>-29</v>
       </c>
-      <c r="N52" s="22">
+      <c r="N52" s="20">
         <v>-29</v>
       </c>
-      <c r="O52" s="22">
+      <c r="O52" s="20">
         <v>-29</v>
       </c>
       <c r="R52">
         <v>2039</v>
       </c>
-      <c r="S52" s="22">
+      <c r="S52" s="20">
         <v>-3</v>
       </c>
-      <c r="T52" s="22">
+      <c r="T52" s="20">
         <v>-3</v>
       </c>
-      <c r="U52" s="22">
+      <c r="U52" s="20">
         <v>-3</v>
       </c>
-      <c r="V52" s="22">
+      <c r="V52" s="20">
         <v>-3</v>
       </c>
-      <c r="W52" s="22">
+      <c r="W52" s="20">
         <v>-3</v>
       </c>
       <c r="AG52" s="15"/>
@@ -58738,19 +58738,19 @@
       <c r="R53">
         <v>2040</v>
       </c>
-      <c r="S53" s="22">
+      <c r="S53" s="20">
         <v>-48</v>
       </c>
-      <c r="T53" s="22">
+      <c r="T53" s="20">
         <v>-29</v>
       </c>
-      <c r="U53" s="22">
+      <c r="U53" s="20">
         <v>-29</v>
       </c>
-      <c r="V53" s="22">
+      <c r="V53" s="20">
         <v>-29</v>
       </c>
-      <c r="W53" s="22">
+      <c r="W53" s="20">
         <v>-29</v>
       </c>
       <c r="AO53" s="15"/>
@@ -59341,30 +59341,30 @@
         <v>2026</v>
       </c>
       <c r="AG64" s="15">
-        <f t="shared" ref="AG64:AG83" si="37">C61/$AC6</f>
+        <f t="shared" ref="AG64:AG81" si="37">C61/$AC6</f>
         <v>-172.0747295968535</v>
       </c>
       <c r="AH64" s="15">
-        <f t="shared" ref="AH64:AH83" si="38">D61/$AC6</f>
+        <f t="shared" ref="AH64:AH81" si="38">D61/$AC6</f>
         <v>-103.2448377581121</v>
       </c>
       <c r="AI64" s="15">
-        <f t="shared" ref="AI64:AI83" si="39">E61/$AC6</f>
+        <f t="shared" ref="AI64:AI81" si="39">E61/$AC6</f>
         <v>-25.565388397246807</v>
       </c>
       <c r="AJ64" s="15">
-        <f t="shared" ref="AJ64:AJ83" si="40">F61/$AC6</f>
+        <f t="shared" ref="AJ64:AJ81" si="40">F61/$AC6</f>
         <v>-37.364798426745331</v>
       </c>
       <c r="AK64" s="15">
-        <f t="shared" ref="AK64:AK83" si="41">G61/$AC6</f>
+        <f t="shared" ref="AK64:AK81" si="41">G61/$AC6</f>
         <v>-103.2448377581121</v>
       </c>
       <c r="AN64">
         <v>2026</v>
       </c>
       <c r="AO64" s="15">
-        <f t="shared" ref="AO64:AO84" si="42">K61/$AC6</f>
+        <f t="shared" ref="AO64:AO82" si="42">K61/$AC6</f>
         <v>-112.094395280236</v>
       </c>
       <c r="AP64" s="15">
@@ -59387,23 +59387,23 @@
         <v>2026</v>
       </c>
       <c r="AW64" s="15">
-        <f t="shared" ref="AW64:AW85" si="43">S61/$AC6</f>
+        <f t="shared" ref="AW64:AW83" si="43">S61/$AC6</f>
         <v>0</v>
       </c>
       <c r="AX64" s="15">
-        <f t="shared" ref="AX64:AX85" si="44">T61/$AC6</f>
+        <f t="shared" ref="AX64:AX83" si="44">T61/$AC6</f>
         <v>0</v>
       </c>
       <c r="AY64" s="15">
-        <f t="shared" ref="AY64:AY85" si="45">U61/$AC6</f>
+        <f t="shared" ref="AY64:AY83" si="45">U61/$AC6</f>
         <v>0</v>
       </c>
       <c r="AZ64" s="15">
-        <f t="shared" ref="AZ64:AZ85" si="46">V61/$AC6</f>
+        <f t="shared" ref="AZ64:AZ83" si="46">V61/$AC6</f>
         <v>0</v>
       </c>
       <c r="BA64" s="15">
-        <f t="shared" ref="BA64:BA85" si="47">W61/$AC6</f>
+        <f t="shared" ref="BA64:BA83" si="47">W61/$AC6</f>
         <v>0</v>
       </c>
     </row>
@@ -61230,19 +61230,19 @@
         <v>8.0365408356673633</v>
       </c>
       <c r="AP79" s="15">
-        <f t="shared" ref="AP79:AP84" si="48">L76/$AC21</f>
+        <f t="shared" ref="AP79:AP82" si="48">L76/$AC21</f>
         <v>5.1141623499701403</v>
       </c>
       <c r="AQ79" s="15">
-        <f t="shared" ref="AQ79:AQ84" si="49">M76/$AC21</f>
+        <f t="shared" ref="AQ79:AQ82" si="49">M76/$AC21</f>
         <v>5.1141623499701403</v>
       </c>
       <c r="AR79" s="15">
-        <f t="shared" ref="AR79:AR84" si="50">N76/$AC21</f>
+        <f t="shared" ref="AR79:AR82" si="50">N76/$AC21</f>
         <v>5.1141623499701403</v>
       </c>
       <c r="AS79" s="15">
-        <f t="shared" ref="AS79:AS84" si="51">O76/$AC21</f>
+        <f t="shared" ref="AS79:AS82" si="51">O76/$AC21</f>
         <v>5.1141623499701403</v>
       </c>
       <c r="AV79">

</xml_diff>